<commit_message>
feat: menu admin completo e refatoração das rotas disponível para consumo da API
</commit_message>
<xml_diff>
--- a/insert_users/alunos.xlsx
+++ b/insert_users/alunos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/39dafe5e34e11193/Documentos/Projetos/Python/cortex/insert_users/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{BE2AA4B0-F5D4-44EF-B097-AE6E1339509F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{020A04B8-625C-4232-AA23-4FDD0B5B7442}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{BE2AA4B0-F5D4-44EF-B097-AE6E1339509F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E79A7B54-B1A3-4398-A268-C1B94929800A}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,10 +89,10 @@
     <t>27/12/2019 00:00:00</t>
   </si>
   <si>
-    <t>Rua Tereza Feitosa, 1881, Nossa Senhora das Gracas, 64519-410, Teresina-PI</t>
-  </si>
-  <si>
     <t>(86) 99999-0000, (86) 99900-0099</t>
+  </si>
+  <si>
+    <t>Rua Tereza Feitosa, 1881B, Nossa Senhora das Gracas, 64519-410, Teresina-PI</t>
   </si>
 </sst>
 </file>
@@ -358,21 +358,21 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
     <col min="4" max="4" width="31.85546875" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="65.5703125" customWidth="1"/>
-    <col min="10" max="10" width="59.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -433,10 +433,10 @@
         <v>33002</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>